<commit_message>
geographicDescription para instead of nonemptyString
</commit_message>
<xml_diff>
--- a/excel-sheets/EBV_terms.xlsx
+++ b/excel-sheets/EBV_terms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christianlanger/Desktop/ebv-reference-guide/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christianlanger/Desktop/DataPortal/ebv-reference-guide/XSD/ebv-profile/excel-sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A68DC71-DEA8-5140-8097-0EFE7C3AF020}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25054CDD-BFD0-134A-98A8-A86B0C8AEB75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="37200" windowHeight="21260" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="16760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Terms" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="Select">measurement!$A$1:$A$4</definedName>
-    <definedName name="Type_of_measurement">Terms!$D$32+measurement!$A:$A</definedName>
+    <definedName name="Type_of_measurement">Terms!$D$38+measurement!$A:$A</definedName>
   </definedNames>
   <calcPr calcId="150000"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="169">
   <si>
     <t>title</t>
   </si>
@@ -630,6 +630,18 @@
   </si>
   <si>
     <t>Not neccessary, EBVname is sufficient ??</t>
+  </si>
+  <si>
+    <t>Remove</t>
+  </si>
+  <si>
+    <t>Color codes:</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Questions?</t>
   </si>
 </sst>
 </file>
@@ -875,7 +887,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
@@ -939,6 +951,12 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20 % - Akzent2" xfId="2" builtinId="34"/>
@@ -1225,27 +1243,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N64"/>
+  <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="22.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="100" style="8" customWidth="1"/>
-    <col min="4" max="4" width="29.1640625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="47" style="8" customWidth="1"/>
-    <col min="6" max="6" width="37.83203125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="32" style="8" customWidth="1"/>
-    <col min="8" max="8" width="32.33203125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="29.1640625" style="8" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="47" style="8" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="8" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="8" customWidth="1"/>
+    <col min="8" max="8" width="31.33203125" style="20" customWidth="1"/>
     <col min="9" max="9" width="26" style="8" customWidth="1"/>
     <col min="10" max="10" width="12.6640625" style="8" customWidth="1"/>
     <col min="11" max="11" width="15.83203125" style="8" customWidth="1"/>
     <col min="12" max="12" width="14.33203125" style="8" customWidth="1"/>
-    <col min="13" max="13" width="31.33203125" style="8" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" style="8" customWidth="1"/>
     <col min="14" max="14" width="53" style="8" customWidth="1"/>
     <col min="15" max="16384" width="10.83203125" style="8"/>
   </cols>
@@ -1294,183 +1312,145 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="30" customFormat="1">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="37" t="s">
+    <row r="2" spans="1:14">
+      <c r="A2" s="63"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="63" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="65"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="66" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="65"/>
+      <c r="N4" s="65"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="67" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="68" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="65"/>
+      <c r="N6" s="65"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="63"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="65"/>
+      <c r="M7" s="65"/>
+      <c r="N7" s="65"/>
+    </row>
+    <row r="8" spans="1:14" s="30" customFormat="1">
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-    </row>
-    <row r="6" spans="1:14" s="28" customFormat="1">
-      <c r="A6" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" s="25"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="62" t="s">
-        <v>44</v>
-      </c>
-      <c r="M6" s="27"/>
-      <c r="N6" s="25" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" s="35" customFormat="1">
-      <c r="A7" s="31" t="s">
-        <v>145</v>
-      </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="32" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" s="28" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25" t="s">
-        <v>146</v>
-      </c>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="5" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="C9" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="D9" s="5"/>
-      <c r="E9" s="5" t="s">
-        <v>99</v>
-      </c>
+      <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="14" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
@@ -1480,19 +1460,21 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="5" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="E10" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="14" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>148</v>
+        <v>0</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -1500,94 +1482,127 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" spans="1:14" s="23" customFormat="1">
-      <c r="A11" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" s="23" customFormat="1">
-      <c r="A12" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="I12" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="K12" s="21" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" s="23" customFormat="1">
-      <c r="A13" s="21"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="40"/>
-      <c r="K13" s="21" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" s="23" customFormat="1">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="40"/>
-      <c r="K14" s="21" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" s="23" customFormat="1">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="40"/>
-      <c r="K15" s="21" t="s">
-        <v>120</v>
-      </c>
+    <row r="11" spans="1:14">
+      <c r="A11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+    </row>
+    <row r="12" spans="1:14" s="28" customFormat="1">
+      <c r="A12" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" s="25"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="M12" s="27"/>
+      <c r="N12" s="25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="35" customFormat="1">
+      <c r="A13" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="32" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="28" customFormat="1" ht="15" customHeight="1">
+      <c r="A14" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="5" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1595,450 +1610,435 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="16" t="s">
-        <v>60</v>
+      <c r="H16" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5" t="s">
+      <c r="N16" s="5"/>
+    </row>
+    <row r="17" spans="1:14" s="23" customFormat="1">
+      <c r="A17" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="23" customFormat="1">
+      <c r="A18" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="K18" s="21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="23" customFormat="1">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="40"/>
+      <c r="K19" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="23" customFormat="1">
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="40"/>
+      <c r="K20" s="21" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="23" customFormat="1">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="40"/>
+      <c r="K21" s="21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="16" t="s">
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I23" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="5" t="s">
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5" t="s">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="15" t="s">
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="I24" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-    </row>
-    <row r="19" spans="1:14" s="21" customFormat="1">
-      <c r="A19" s="38" t="s">
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+    </row>
+    <row r="25" spans="1:14" s="21" customFormat="1">
+      <c r="A25" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="39" t="s">
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="I19" s="38" t="s">
+      <c r="I25" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="38"/>
-      <c r="N19" s="38" t="s">
+      <c r="J25" s="38"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="38" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="5" customFormat="1">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-    </row>
-    <row r="21" spans="1:14" s="47" customFormat="1">
-      <c r="A21" s="44" t="s">
+    <row r="26" spans="1:14" s="5" customFormat="1">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+    </row>
+    <row r="27" spans="1:14" s="47" customFormat="1">
+      <c r="A27" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="B21" s="45"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="48" t="s">
+      <c r="B27" s="45"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="J21" s="45"/>
-      <c r="K21" s="45"/>
-      <c r="L21" s="45"/>
-      <c r="M21" s="45"/>
-      <c r="N21" s="45"/>
-    </row>
-    <row r="22" spans="1:14" s="25" customFormat="1">
-      <c r="A22" s="41"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="24" t="s">
+      <c r="J27" s="45"/>
+      <c r="K27" s="45"/>
+      <c r="L27" s="45"/>
+      <c r="M27" s="45"/>
+      <c r="N27" s="45"/>
+    </row>
+    <row r="28" spans="1:14" s="25" customFormat="1">
+      <c r="A28" s="41"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="K22" s="25" t="s">
+      <c r="K28" s="25" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="25" customFormat="1">
-      <c r="A23" s="41"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="24" t="s">
+    <row r="29" spans="1:14" s="25" customFormat="1">
+      <c r="A29" s="41"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="K23" s="25" t="s">
+      <c r="K29" s="25" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:14" s="25" customFormat="1">
-      <c r="A24" s="41"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="24" t="s">
+    <row r="30" spans="1:14" s="25" customFormat="1">
+      <c r="A30" s="41"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="K24" s="25" t="s">
+      <c r="K30" s="25" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="25" customFormat="1">
-      <c r="A25" s="41"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="24" t="s">
+    <row r="31" spans="1:14" s="25" customFormat="1">
+      <c r="A31" s="41"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="K25" s="25" t="s">
+      <c r="K31" s="25" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="58" customFormat="1">
-      <c r="A26" s="57"/>
-      <c r="H26" s="59"/>
-    </row>
-    <row r="27" spans="1:14" s="47" customFormat="1">
-      <c r="A27" s="51"/>
-      <c r="H27" s="52"/>
-      <c r="I27" s="37" t="s">
+    <row r="32" spans="1:14" s="58" customFormat="1">
+      <c r="A32" s="57"/>
+      <c r="H32" s="59"/>
+    </row>
+    <row r="33" spans="1:14" s="47" customFormat="1">
+      <c r="A33" s="51"/>
+      <c r="H33" s="52"/>
+      <c r="I33" s="37" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="21" customFormat="1">
-      <c r="A28" s="21" t="s">
+    <row r="34" spans="1:14" s="21" customFormat="1">
+      <c r="A34" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C34" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E34" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="H28" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="I28" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="N28" s="21" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" s="21" customFormat="1">
-      <c r="A29" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="H29" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="I29" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="N29" s="21" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" s="5" customFormat="1">
-      <c r="H30" s="11"/>
-    </row>
-    <row r="31" spans="1:14" s="47" customFormat="1">
-      <c r="H31" s="50"/>
-      <c r="I31" s="37" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" s="23" customFormat="1">
-      <c r="A32" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="D32" s="49"/>
-      <c r="E32" s="49" t="s">
-        <v>97</v>
-      </c>
-      <c r="F32" s="49"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
-      <c r="K32" s="21"/>
-      <c r="L32" s="21"/>
-      <c r="M32" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="N32" s="21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" s="23" customFormat="1">
-      <c r="A33" s="21"/>
-      <c r="B33" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
-      <c r="L33" s="21"/>
-      <c r="M33" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="N33" s="21"/>
-    </row>
-    <row r="34" spans="1:14" s="23" customFormat="1">
-      <c r="A34" s="21"/>
-      <c r="B34" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="C34" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
       <c r="H34" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="21"/>
-      <c r="L34" s="21"/>
-      <c r="M34" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="N34" s="21"/>
-    </row>
-    <row r="35" spans="1:14">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="N35" s="5"/>
-    </row>
-    <row r="36" spans="1:14">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="N36" s="5"/>
-    </row>
-    <row r="37" spans="1:14">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
-    </row>
-    <row r="38" spans="1:14" s="30" customFormat="1">
-      <c r="A38" s="47"/>
-      <c r="B38" s="47"/>
-      <c r="C38" s="47"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="47"/>
-      <c r="H38" s="50"/>
-      <c r="I38" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="J38" s="47"/>
-      <c r="K38" s="47"/>
-      <c r="L38" s="47"/>
-      <c r="M38" s="47"/>
-      <c r="N38" s="47"/>
+      <c r="I34" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="N34" s="21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" s="21" customFormat="1">
+      <c r="A35" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="H35" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="I35" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="N35" s="21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" s="5" customFormat="1">
+      <c r="H36" s="11"/>
+    </row>
+    <row r="37" spans="1:14" s="47" customFormat="1">
+      <c r="H37" s="50"/>
+      <c r="I37" s="37" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" s="23" customFormat="1">
+      <c r="A38" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="F38" s="49"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="N38" s="21" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="39" spans="1:14" s="23" customFormat="1">
-      <c r="A39" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B39" s="21"/>
+      <c r="A39" s="21"/>
+      <c r="B39" s="21" t="s">
+        <v>81</v>
+      </c>
       <c r="C39" s="21"/>
       <c r="D39" s="21"/>
       <c r="E39" s="21"/>
       <c r="F39" s="21"/>
       <c r="G39" s="21"/>
-      <c r="H39" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="I39" s="21" t="s">
-        <v>111</v>
-      </c>
+      <c r="H39" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="I39" s="21"/>
       <c r="J39" s="21"/>
       <c r="K39" s="21"/>
       <c r="L39" s="21"/>
-      <c r="M39" s="21"/>
+      <c r="M39" s="21" t="s">
+        <v>131</v>
+      </c>
       <c r="N39" s="21"/>
     </row>
     <row r="40" spans="1:14" s="23" customFormat="1">
       <c r="A40" s="21"/>
       <c r="B40" s="21" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="D40" s="21"/>
       <c r="E40" s="21"/>
       <c r="F40" s="21"/>
       <c r="G40" s="21"/>
-      <c r="H40" s="40" t="s">
-        <v>55</v>
+      <c r="H40" s="43" t="s">
+        <v>50</v>
       </c>
       <c r="I40" s="21"/>
       <c r="J40" s="21"/>
       <c r="K40" s="21"/>
       <c r="L40" s="21"/>
-      <c r="M40" s="21"/>
+      <c r="M40" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="N40" s="21"/>
     </row>
-    <row r="41" spans="1:14" s="23" customFormat="1">
-      <c r="A41" s="21"/>
-      <c r="B41" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C41" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="21"/>
-      <c r="L41" s="21"/>
-      <c r="M41" s="21"/>
-      <c r="N41" s="21"/>
-    </row>
-    <row r="42" spans="1:14" s="23" customFormat="1">
-      <c r="A42" s="21"/>
-      <c r="B42" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
-      <c r="K42" s="21"/>
-      <c r="L42" s="21"/>
-      <c r="M42" s="21"/>
-      <c r="N42" s="21"/>
+    <row r="41" spans="1:14">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="N41" s="5"/>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="N42" s="5"/>
     </row>
     <row r="43" spans="1:14">
       <c r="A43" s="5"/>
@@ -2048,7 +2048,7 @@
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
-      <c r="H43" s="9"/>
+      <c r="H43" s="18"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
       <c r="K43" s="5"/>
@@ -2064,9 +2064,9 @@
       <c r="E44" s="47"/>
       <c r="F44" s="47"/>
       <c r="G44" s="47"/>
-      <c r="H44" s="53"/>
+      <c r="H44" s="50"/>
       <c r="I44" s="37" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="J44" s="47"/>
       <c r="K44" s="47"/>
@@ -2074,225 +2074,207 @@
       <c r="M44" s="47"/>
       <c r="N44" s="47"/>
     </row>
-    <row r="45" spans="1:14" s="25" customFormat="1">
-      <c r="A45" s="55" t="s">
+    <row r="45" spans="1:14" s="23" customFormat="1">
+      <c r="A45" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="I45" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="J45" s="21"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="21"/>
+      <c r="M45" s="21"/>
+      <c r="N45" s="21"/>
+    </row>
+    <row r="46" spans="1:14" s="23" customFormat="1">
+      <c r="A46" s="21"/>
+      <c r="B46" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="21"/>
+      <c r="N46" s="21"/>
+    </row>
+    <row r="47" spans="1:14" s="23" customFormat="1">
+      <c r="A47" s="21"/>
+      <c r="B47" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="I47" s="21"/>
+      <c r="J47" s="21"/>
+      <c r="K47" s="21"/>
+      <c r="L47" s="21"/>
+      <c r="M47" s="21"/>
+      <c r="N47" s="21"/>
+    </row>
+    <row r="48" spans="1:14" s="23" customFormat="1">
+      <c r="A48" s="21"/>
+      <c r="B48" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="I48" s="21"/>
+      <c r="J48" s="21"/>
+      <c r="K48" s="21"/>
+      <c r="L48" s="21"/>
+      <c r="M48" s="21"/>
+      <c r="N48" s="21"/>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="5"/>
+    </row>
+    <row r="50" spans="1:14" s="30" customFormat="1">
+      <c r="A50" s="47"/>
+      <c r="B50" s="47"/>
+      <c r="C50" s="47"/>
+      <c r="D50" s="47"/>
+      <c r="E50" s="47"/>
+      <c r="F50" s="47"/>
+      <c r="G50" s="47"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="J50" s="47"/>
+      <c r="K50" s="47"/>
+      <c r="L50" s="47"/>
+      <c r="M50" s="47"/>
+      <c r="N50" s="47"/>
+    </row>
+    <row r="51" spans="1:14" s="25" customFormat="1">
+      <c r="A51" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="B45" s="55"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="55"/>
-      <c r="E45" s="55"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="55"/>
-      <c r="H45" s="61" t="s">
+      <c r="B51" s="55"/>
+      <c r="C51" s="55"/>
+      <c r="D51" s="55"/>
+      <c r="E51" s="55"/>
+      <c r="F51" s="55"/>
+      <c r="G51" s="55"/>
+      <c r="H51" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="I45" s="55" t="s">
+      <c r="I51" s="55" t="s">
         <v>112</v>
       </c>
-      <c r="J45" s="55"/>
-      <c r="K45" s="55"/>
-      <c r="L45" s="55"/>
-      <c r="M45" s="55"/>
-      <c r="N45" s="55" t="s">
+      <c r="J51" s="55"/>
+      <c r="K51" s="55"/>
+      <c r="L51" s="55"/>
+      <c r="M51" s="55"/>
+      <c r="N51" s="55" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="46" spans="1:14" s="5" customFormat="1">
-      <c r="H46" s="9"/>
-    </row>
-    <row r="47" spans="1:14" s="47" customFormat="1">
-      <c r="H47" s="53"/>
-      <c r="I47" s="37" t="s">
+    <row r="52" spans="1:14" s="5" customFormat="1">
+      <c r="H52" s="9"/>
+    </row>
+    <row r="53" spans="1:14" s="47" customFormat="1">
+      <c r="H53" s="53"/>
+      <c r="I53" s="37" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="48" spans="1:14" s="25" customFormat="1">
-      <c r="A48" s="25" t="s">
+    <row r="54" spans="1:14" s="25" customFormat="1">
+      <c r="A54" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="C48" s="25" t="s">
+      <c r="C54" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="E48" s="25" t="s">
+      <c r="E54" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="H48" s="60" t="s">
+      <c r="H54" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="J48" s="25" t="s">
+      <c r="J54" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="N48" s="25" t="s">
+      <c r="N54" s="25" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="49" spans="1:14" s="5" customFormat="1">
-      <c r="H49" s="11"/>
-    </row>
-    <row r="50" spans="1:14" s="47" customFormat="1">
-      <c r="H50" s="50"/>
-      <c r="I50" s="37" t="s">
+    <row r="55" spans="1:14" s="5" customFormat="1">
+      <c r="H55" s="11"/>
+    </row>
+    <row r="56" spans="1:14" s="47" customFormat="1">
+      <c r="H56" s="50"/>
+      <c r="I56" s="37" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="51" spans="1:14">
-      <c r="A51" s="5" t="s">
+    <row r="57" spans="1:14">
+      <c r="A57" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5" t="s">
+      <c r="B57" s="5"/>
+      <c r="C57" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="J51" s="5"/>
-      <c r="K51" s="5"/>
-      <c r="L51" s="5"/>
-      <c r="M51" s="5"/>
-      <c r="N51" s="5"/>
-    </row>
-    <row r="52" spans="1:14">
-      <c r="A52" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H52" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="J52" s="5"/>
-      <c r="K52" s="5"/>
-      <c r="L52" s="5"/>
-      <c r="M52" s="5"/>
-      <c r="N52" s="5"/>
-    </row>
-    <row r="53" spans="1:14">
-      <c r="A53" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
-      <c r="K53" s="5"/>
-      <c r="L53" s="5"/>
-      <c r="M53" s="5"/>
-      <c r="N53" s="5"/>
-    </row>
-    <row r="54" spans="1:14">
-      <c r="A54" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="J54" s="5"/>
-      <c r="K54" s="5"/>
-      <c r="L54" s="5"/>
-      <c r="M54" s="5"/>
-      <c r="N54" s="5"/>
-    </row>
-    <row r="55" spans="1:14">
-      <c r="A55" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="G55" s="5"/>
-      <c r="H55" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="I55" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="J55" s="5"/>
-      <c r="K55" s="5"/>
-      <c r="L55" s="5"/>
-      <c r="M55" s="5"/>
-      <c r="N55" s="5"/>
-    </row>
-    <row r="56" spans="1:14">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="5"/>
-      <c r="H56" s="16"/>
-      <c r="I56" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="J56" s="5"/>
-      <c r="K56" s="5"/>
-      <c r="L56" s="5"/>
-      <c r="M56" s="5"/>
-      <c r="N56" s="5"/>
-    </row>
-    <row r="57" spans="1:14">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
-      <c r="H57" s="16"/>
+      <c r="H57" s="16" t="s">
+        <v>49</v>
+      </c>
       <c r="I57" s="5" t="s">
-        <v>83</v>
+        <v>155</v>
       </c>
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
@@ -2301,138 +2283,278 @@
       <c r="N57" s="5"/>
     </row>
     <row r="58" spans="1:14">
-      <c r="A58" s="5"/>
+      <c r="A58" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
+      <c r="C58" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="5"/>
+      <c r="G58" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H58" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>156</v>
+      </c>
       <c r="J58" s="5"/>
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
       <c r="M58" s="5"/>
       <c r="N58" s="5"/>
     </row>
-    <row r="59" spans="1:14" s="30" customFormat="1">
-      <c r="A59" s="47"/>
-      <c r="B59" s="47"/>
-      <c r="C59" s="47"/>
-      <c r="D59" s="47"/>
-      <c r="E59" s="47"/>
-      <c r="F59" s="47"/>
-      <c r="G59" s="47"/>
-      <c r="H59" s="53"/>
-      <c r="I59" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="J59" s="47"/>
-      <c r="K59" s="47"/>
-      <c r="L59" s="47"/>
-      <c r="M59" s="47"/>
-      <c r="N59" s="47"/>
-    </row>
-    <row r="60" spans="1:14" s="23" customFormat="1">
-      <c r="A60" s="54" t="s">
-        <v>33</v>
-      </c>
-      <c r="B60" s="21"/>
-      <c r="C60" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D60" s="21"/>
-      <c r="E60" s="21"/>
-      <c r="F60" s="21"/>
-      <c r="G60" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="H60" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="I60" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="J60" s="21"/>
-      <c r="K60" s="21"/>
-      <c r="L60" s="21"/>
-      <c r="M60" s="21"/>
-      <c r="N60" s="21" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" s="23" customFormat="1">
-      <c r="A61" s="54"/>
-      <c r="B61" s="21"/>
-      <c r="C61" s="21"/>
-      <c r="D61" s="21"/>
-      <c r="E61" s="21"/>
-      <c r="F61" s="21"/>
-      <c r="G61" s="21"/>
-      <c r="H61" s="43"/>
-      <c r="I61" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="J61" s="21"/>
-      <c r="K61" s="21"/>
-      <c r="L61" s="21"/>
-      <c r="M61" s="21"/>
-      <c r="N61" s="21"/>
-    </row>
-    <row r="62" spans="1:14" s="23" customFormat="1">
-      <c r="A62" s="54"/>
-      <c r="B62" s="21"/>
-      <c r="C62" s="21"/>
-      <c r="D62" s="21"/>
-      <c r="E62" s="21"/>
-      <c r="F62" s="21"/>
-      <c r="G62" s="21"/>
-      <c r="H62" s="43"/>
-      <c r="I62" s="21"/>
-      <c r="J62" s="21"/>
-      <c r="K62" s="21"/>
-      <c r="L62" s="21"/>
-      <c r="M62" s="21"/>
-      <c r="N62" s="21"/>
+    <row r="59" spans="1:14">
+      <c r="A59" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="5"/>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="A60" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="I60" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="J60" s="5"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
+      <c r="M60" s="5"/>
+      <c r="N60" s="5"/>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="A61" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G61" s="5"/>
+      <c r="H61" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="I61" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="J61" s="5"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5"/>
+      <c r="M61" s="5"/>
+      <c r="N61" s="5"/>
+    </row>
+    <row r="62" spans="1:14">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="16"/>
+      <c r="I62" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="J62" s="5"/>
+      <c r="K62" s="5"/>
+      <c r="L62" s="5"/>
+      <c r="M62" s="5"/>
+      <c r="N62" s="5"/>
     </row>
     <row r="63" spans="1:14">
-      <c r="A63" s="12"/>
-      <c r="B63" s="5"/>
+      <c r="A63" s="5"/>
+      <c r="B63" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
-      <c r="H63" s="11"/>
-      <c r="I63" s="5"/>
+      <c r="H63" s="16"/>
+      <c r="I63" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="J63" s="5"/>
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
       <c r="M63" s="5"/>
       <c r="N63" s="5"/>
     </row>
-    <row r="64" spans="1:14" s="28" customFormat="1">
-      <c r="A64" s="55" t="s">
+    <row r="64" spans="1:14">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="16"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
+      <c r="K64" s="5"/>
+      <c r="L64" s="5"/>
+      <c r="M64" s="5"/>
+      <c r="N64" s="5"/>
+    </row>
+    <row r="65" spans="1:14" s="30" customFormat="1">
+      <c r="A65" s="47"/>
+      <c r="B65" s="47"/>
+      <c r="C65" s="47"/>
+      <c r="D65" s="47"/>
+      <c r="E65" s="47"/>
+      <c r="F65" s="47"/>
+      <c r="G65" s="47"/>
+      <c r="H65" s="53"/>
+      <c r="I65" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="J65" s="47"/>
+      <c r="K65" s="47"/>
+      <c r="L65" s="47"/>
+      <c r="M65" s="47"/>
+      <c r="N65" s="47"/>
+    </row>
+    <row r="66" spans="1:14" s="23" customFormat="1">
+      <c r="A66" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="B66" s="21"/>
+      <c r="C66" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D66" s="21"/>
+      <c r="E66" s="21"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H66" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="I66" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="J66" s="21"/>
+      <c r="K66" s="21"/>
+      <c r="L66" s="21"/>
+      <c r="M66" s="21"/>
+      <c r="N66" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" s="23" customFormat="1">
+      <c r="A67" s="54"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="21"/>
+      <c r="G67" s="21"/>
+      <c r="H67" s="43"/>
+      <c r="I67" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="J67" s="21"/>
+      <c r="K67" s="21"/>
+      <c r="L67" s="21"/>
+      <c r="M67" s="21"/>
+      <c r="N67" s="21"/>
+    </row>
+    <row r="68" spans="1:14" s="23" customFormat="1">
+      <c r="A68" s="54"/>
+      <c r="B68" s="21"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="21"/>
+      <c r="E68" s="21"/>
+      <c r="F68" s="21"/>
+      <c r="G68" s="21"/>
+      <c r="H68" s="43"/>
+      <c r="I68" s="21"/>
+      <c r="J68" s="21"/>
+      <c r="K68" s="21"/>
+      <c r="L68" s="21"/>
+      <c r="M68" s="21"/>
+      <c r="N68" s="21"/>
+    </row>
+    <row r="69" spans="1:14">
+      <c r="A69" s="12"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="11"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="5"/>
+      <c r="K69" s="5"/>
+      <c r="L69" s="5"/>
+      <c r="M69" s="5"/>
+      <c r="N69" s="5"/>
+    </row>
+    <row r="70" spans="1:14" s="28" customFormat="1">
+      <c r="A70" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="B64" s="55"/>
-      <c r="C64" s="55" t="s">
+      <c r="B70" s="55"/>
+      <c r="C70" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="D64" s="55"/>
-      <c r="E64" s="55"/>
-      <c r="F64" s="55"/>
-      <c r="G64" s="55"/>
-      <c r="H64" s="56" t="s">
+      <c r="D70" s="55"/>
+      <c r="E70" s="55"/>
+      <c r="F70" s="55"/>
+      <c r="G70" s="55"/>
+      <c r="H70" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="I64" s="55"/>
-      <c r="J64" s="55"/>
-      <c r="K64" s="55"/>
-      <c r="L64" s="55"/>
-      <c r="M64" s="55"/>
-      <c r="N64" s="55" t="s">
+      <c r="I70" s="55"/>
+      <c r="J70" s="55"/>
+      <c r="K70" s="55"/>
+      <c r="L70" s="55"/>
+      <c r="M70" s="55"/>
+      <c r="N70" s="55" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2445,7 +2567,7 @@
           <x14:formula1>
             <xm:f>measurement!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>D32</xm:sqref>
+          <xm:sqref>D38</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
add measurement elements based on call discussion 21/06/2019
</commit_message>
<xml_diff>
--- a/excel-sheets/EBV_terms.xlsx
+++ b/excel-sheets/EBV_terms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christianlanger/Desktop/DataPortal/ebv-reference-guide/XSD/ebv-profile/excel-sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25054CDD-BFD0-134A-98A8-A86B0C8AEB75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF789C8-F25A-E342-888E-4A68A3A301FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="16760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1120" yWindow="740" windowWidth="36800" windowHeight="20220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Terms" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="172">
   <si>
     <t>title</t>
   </si>
@@ -642,6 +642,15 @@
   </si>
   <si>
     <t>Questions?</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>forest cover/Body mass</t>
+  </si>
+  <si>
+    <t>percentage/grams</t>
   </si>
 </sst>
 </file>
@@ -752,7 +761,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -830,6 +839,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -887,7 +902,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
@@ -949,7 +964,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -957,6 +971,9 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20 % - Akzent2" xfId="2" builtinId="34"/>
@@ -1245,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1263,7 +1280,7 @@
     <col min="10" max="10" width="12.6640625" style="8" customWidth="1"/>
     <col min="11" max="11" width="15.83203125" style="8" customWidth="1"/>
     <col min="12" max="12" width="14.33203125" style="8" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" style="8" customWidth="1"/>
+    <col min="13" max="13" width="24" style="8" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="53" style="8" customWidth="1"/>
     <col min="15" max="16384" width="10.83203125" style="8"/>
   </cols>
@@ -1313,108 +1330,108 @@
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="63"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
+      <c r="A2" s="62"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="62" t="s">
         <v>166</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="65" t="s">
         <v>165</v>
       </c>
-      <c r="B4" s="63"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="63"/>
-      <c r="J4" s="63"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65"/>
-      <c r="M4" s="65"/>
-      <c r="N4" s="65"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="64"/>
+      <c r="N4" s="64"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="66" t="s">
         <v>167</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="64"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="67" t="s">
         <v>168</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="63"/>
-      <c r="J6" s="63"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="65"/>
-      <c r="M6" s="65"/>
-      <c r="N6" s="65"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="64"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="63"/>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="64"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="65"/>
-      <c r="L7" s="65"/>
-      <c r="M7" s="65"/>
-      <c r="N7" s="65"/>
+      <c r="A7" s="62"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="64"/>
+      <c r="M7" s="64"/>
+      <c r="N7" s="64"/>
     </row>
     <row r="8" spans="1:14" s="30" customFormat="1">
       <c r="A8" s="29"/>
@@ -1520,7 +1537,7 @@
       <c r="I12" s="25"/>
       <c r="J12" s="27"/>
       <c r="K12" s="27"/>
-      <c r="L12" s="62" t="s">
+      <c r="L12" s="61" t="s">
         <v>44</v>
       </c>
       <c r="M12" s="27"/>
@@ -1963,7 +1980,9 @@
       <c r="B39" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="C39" s="21"/>
+      <c r="C39" s="21" t="s">
+        <v>171</v>
+      </c>
       <c r="D39" s="21"/>
       <c r="E39" s="21"/>
       <c r="F39" s="21"/>
@@ -2006,8 +2025,12 @@
     </row>
     <row r="41" spans="1:14">
       <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
+      <c r="B41" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>170</v>
+      </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -2196,27 +2219,27 @@
       <c r="M50" s="47"/>
       <c r="N50" s="47"/>
     </row>
-    <row r="51" spans="1:14" s="25" customFormat="1">
-      <c r="A51" s="55" t="s">
+    <row r="51" spans="1:14" s="70" customFormat="1">
+      <c r="A51" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="B51" s="55"/>
-      <c r="C51" s="55"/>
-      <c r="D51" s="55"/>
-      <c r="E51" s="55"/>
-      <c r="F51" s="55"/>
-      <c r="G51" s="55"/>
-      <c r="H51" s="61" t="s">
+      <c r="B51" s="68"/>
+      <c r="C51" s="68"/>
+      <c r="D51" s="68"/>
+      <c r="E51" s="68"/>
+      <c r="F51" s="68"/>
+      <c r="G51" s="68"/>
+      <c r="H51" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="I51" s="55" t="s">
+      <c r="I51" s="68" t="s">
         <v>112</v>
       </c>
-      <c r="J51" s="55"/>
-      <c r="K51" s="55"/>
-      <c r="L51" s="55"/>
-      <c r="M51" s="55"/>
-      <c r="N51" s="55" t="s">
+      <c r="J51" s="68"/>
+      <c r="K51" s="68"/>
+      <c r="L51" s="68"/>
+      <c r="M51" s="68"/>
+      <c r="N51" s="68" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2632,12 +2655,12 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection sqref="A1:A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="119.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="135" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">

</xml_diff>